<commit_message>
chore: Actualizar Curva S
</commit_message>
<xml_diff>
--- a/Curva S Gisee.xlsx
+++ b/Curva S Gisee.xlsx
@@ -67,7 +67,7 @@
     <t>Implementación de autenticación y registro de conversaciones</t>
   </si>
   <si>
-    <t>Módulo de memoria contextual + consultas por fecha</t>
+    <t>Módulo de memoria contextual + consultas por usuario</t>
   </si>
   <si>
     <t>Exportación de reportes PDF/Excel + dashboard psicólogos</t>
@@ -76,7 +76,7 @@
     <t>Análisis de emociones (texto/voz) + integración en flujo</t>
   </si>
   <si>
-    <t>Optimización de rendimiento + seguridad básica (bcrypt/SSL)</t>
+    <t>Optimización de rendimiento + seguridad básica (bcrypt/SSL) + Integración hardware</t>
   </si>
   <si>
     <t>Pruebas, validaciones finales y documentación entregable</t>
@@ -844,19 +844,19 @@
         <v>12.0</v>
       </c>
       <c r="F4" s="13">
-        <f t="shared" ref="F4:F6" si="2">D4-C4</f>
+        <f t="shared" ref="F4:F10" si="2">D4-C4</f>
         <v>-2</v>
       </c>
       <c r="G4" s="13">
-        <f t="shared" ref="G4:G6" si="3">D4-E4</f>
+        <f t="shared" ref="G4:G10" si="3">D4-E4</f>
         <v>-4</v>
       </c>
       <c r="H4" s="14">
-        <f t="shared" ref="H4:H6" si="4">D4/C4</f>
+        <f t="shared" ref="H4:H10" si="4">D4/C4</f>
         <v>0.8</v>
       </c>
       <c r="I4" s="14">
-        <f t="shared" ref="I4:I6" si="5">D4/E4</f>
+        <f t="shared" ref="I4:I10" si="5">D4/E4</f>
         <v>0.6666666667</v>
       </c>
       <c r="J4" s="1"/>
@@ -1008,11 +1008,28 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="D7" s="12">
+        <v>44.0</v>
+      </c>
+      <c r="E7" s="12">
+        <v>40.0</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="4"/>
+        <v>0.9777777778</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="5"/>
+        <v>1.1</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="M7" s="15">
@@ -1048,12 +1065,28 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="D8" s="12">
+        <v>61.0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>60.0</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="4"/>
+        <v>1.016666667</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="5"/>
+        <v>1.016666667</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="M8" s="15">
@@ -1089,12 +1122,28 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="D9" s="12">
+        <v>72.0</v>
+      </c>
+      <c r="E9" s="12">
+        <v>70.0</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="4"/>
+        <v>1.028571429</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="5"/>
+        <v>1.028571429</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="M9" s="15">
@@ -1130,12 +1179,28 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="D10" s="12">
+        <v>80.0</v>
+      </c>
+      <c r="E10" s="12">
+        <v>79.0</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="5"/>
+        <v>1.012658228</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="M10" s="15">
@@ -1173,10 +1238,10 @@
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="M11" s="15">
@@ -1214,10 +1279,10 @@
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="M12" s="15">

</xml_diff>